<commit_message>
updated work on business stats
</commit_message>
<xml_diff>
--- a/business Stats/Book1.xlsx
+++ b/business Stats/Book1.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Ujwal\git\business Stats\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B51AB93A-4BEF-4956-83C9-A78CB05382C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA68C356-FBA2-4F64-ACD6-C46FC28182DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{84D76DE3-8557-4722-B5C1-4893E077E0C2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{84D76DE3-8557-4722-B5C1-4893E077E0C2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="35">
   <si>
     <t>Calculate the correlation of the following data</t>
   </si>
@@ -104,13 +105,43 @@
   </si>
   <si>
     <t>Regression equation</t>
+  </si>
+  <si>
+    <t>1.2209x+0.6279</t>
+  </si>
+  <si>
+    <t>f</t>
+  </si>
+  <si>
+    <t>fx</t>
+  </si>
+  <si>
+    <t>mean</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>q</t>
+  </si>
+  <si>
+    <t>np</t>
+  </si>
+  <si>
+    <t>p(x)</t>
+  </si>
+  <si>
+    <t>EF</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="0.0000"/>
+  </numFmts>
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -132,6 +163,13 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="15"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -141,7 +179,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -149,20 +187,262 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1438,41 +1718,41 @@
   <dimension ref="A1:K19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+      <selection activeCell="K24" sqref="K24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.77734375" customWidth="1"/>
-    <col min="2" max="2" width="11.33203125" customWidth="1"/>
-    <col min="3" max="3" width="11.44140625" customWidth="1"/>
-    <col min="4" max="4" width="11.21875" customWidth="1"/>
-    <col min="11" max="11" width="13.33203125" customWidth="1"/>
+    <col min="1" max="1" width="8.7109375" customWidth="1"/>
+    <col min="2" max="2" width="11.28515625" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" customWidth="1"/>
+    <col min="11" max="11" width="13.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="8"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="8"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -1492,7 +1772,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -1511,12 +1791,12 @@
       <c r="F4">
         <v>5</v>
       </c>
-      <c r="I4" s="2" t="s">
+      <c r="I4" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="J4" s="1"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J4" s="8"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="J5" t="s">
         <v>19</v>
       </c>
@@ -1524,15 +1804,15 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
+      <c r="B6" s="8"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
       <c r="J6" t="s">
         <v>21</v>
       </c>
@@ -1540,23 +1820,23 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A8" s="2" t="s">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="1"/>
-      <c r="F8" s="2" t="s">
+      <c r="B8" s="8"/>
+      <c r="F8" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="G8" s="1"/>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
+      <c r="G8" s="8"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
+      <c r="B9" s="8"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
       <c r="F9" t="s">
         <v>1</v>
       </c>
@@ -1564,11 +1844,11 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="8"/>
+      <c r="B10" s="8"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
       <c r="F10">
         <v>2</v>
       </c>
@@ -1576,26 +1856,26 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A11" s="1" t="s">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
+      <c r="B11" s="8"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
       <c r="F11">
         <v>7</v>
       </c>
       <c r="G11">
         <v>9</v>
       </c>
-      <c r="K11" s="4"/>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
+      <c r="K11" s="2"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="8"/>
+      <c r="B12" s="8"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
       <c r="F12">
         <v>6</v>
       </c>
@@ -1603,13 +1883,13 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A13" s="1">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="8">
         <v>3</v>
       </c>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
+      <c r="B13" s="8"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
       <c r="F13">
         <v>3</v>
       </c>
@@ -1617,11 +1897,11 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="8"/>
+      <c r="B14" s="8"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
       <c r="F14">
         <v>4</v>
       </c>
@@ -1629,7 +1909,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="F16" t="s">
         <v>7</v>
       </c>
@@ -1638,19 +1918,19 @@
         <v>0.92447345164190509</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" s="3" t="s">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A19" s="1" t="s">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
+      <c r="B19" s="8"/>
+      <c r="C19" s="8"/>
+      <c r="D19" s="8"/>
+      <c r="E19" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -1673,29 +1953,32 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FFF9418-610B-4438-8F31-62DA5DBBBE22}">
   <dimension ref="A2:G37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O41" sqref="O41"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Q25" sqref="Q25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="15.140625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B2" s="1" t="s">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B2" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B3" s="8"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>1</v>
       </c>
@@ -1715,7 +1998,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>2</v>
       </c>
@@ -1735,33 +2018,33 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B7" s="1" t="s">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B7" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" s="2" t="s">
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="1"/>
-      <c r="E10" s="2" t="s">
+      <c r="B10" s="8"/>
+      <c r="E10" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="F10" s="2"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" s="1" t="s">
+      <c r="F10" s="9"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
+      <c r="B11" s="8"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
       <c r="E11" t="s">
         <v>1</v>
       </c>
@@ -1769,13 +2052,13 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" s="1" t="s">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
+      <c r="B12" s="8"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
       <c r="E12">
         <v>2</v>
       </c>
@@ -1783,13 +2066,13 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" s="1" t="s">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
+      <c r="B13" s="8"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
       <c r="E13">
         <v>7</v>
       </c>
@@ -1797,7 +2080,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E14">
         <v>6</v>
       </c>
@@ -1805,7 +2088,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E15">
         <v>3</v>
       </c>
@@ -1813,7 +2096,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E16">
         <v>4</v>
       </c>
@@ -1821,17 +2104,17 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="5:6" x14ac:dyDescent="0.3">
-      <c r="E18" s="1" t="s">
+    <row r="18" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E18" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="F18" s="1"/>
-    </row>
-    <row r="19" spans="5:6" x14ac:dyDescent="0.3">
-      <c r="E19" s="1"/>
-      <c r="F19" s="1"/>
-    </row>
-    <row r="20" spans="5:6" x14ac:dyDescent="0.3">
+      <c r="F18" s="8"/>
+    </row>
+    <row r="19" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E19" s="8"/>
+      <c r="F19" s="8"/>
+    </row>
+    <row r="20" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E20" t="s">
         <v>24</v>
       </c>
@@ -1840,17 +2123,20 @@
         <v>12.819999999999999</v>
       </c>
     </row>
-    <row r="36" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B36" s="2" t="s">
+    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B36" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C36" s="1"/>
-    </row>
-    <row r="37" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B37" s="1" t="s">
+      <c r="C36" s="8"/>
+    </row>
+    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B37" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C37" s="1"/>
+      <c r="C37" s="8"/>
+      <c r="D37" t="s">
+        <v>26</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="10">
@@ -1869,4 +2155,308 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68AC71F3-EDAC-4C28-A1D6-182EE705764F}">
+  <dimension ref="A4:H27"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="L20" sqref="L20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="4" spans="1:8" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+    </row>
+    <row r="5" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="8"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+    </row>
+    <row r="6" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="1"/>
+    </row>
+    <row r="7" spans="1:8" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="E7" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="F7" s="25" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="B8" s="10">
+        <v>0</v>
+      </c>
+      <c r="C8" s="11">
+        <v>10</v>
+      </c>
+      <c r="D8" s="12">
+        <f>B8*C8</f>
+        <v>0</v>
+      </c>
+      <c r="E8" s="23">
+        <f>_xlfn.BINOM.DIST(B8,5,0.43,0)</f>
+        <v>6.016920570000004E-2</v>
+      </c>
+      <c r="F8" s="26">
+        <f>67*E8</f>
+        <v>4.031336781900003</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="B9" s="4">
+        <v>1</v>
+      </c>
+      <c r="C9" s="6">
+        <v>12</v>
+      </c>
+      <c r="D9" s="12">
+        <f t="shared" ref="D9:D13" si="0">B9*C9</f>
+        <v>12</v>
+      </c>
+      <c r="E9" s="22">
+        <f t="shared" ref="E9:E13" si="1">_xlfn.BINOM.DIST(B9,5,0.43,0)</f>
+        <v>0.22695402150000005</v>
+      </c>
+      <c r="F9" s="26">
+        <f t="shared" ref="F9:F13" si="2">67*E9</f>
+        <v>15.205919440500002</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="B10" s="4">
+        <v>2</v>
+      </c>
+      <c r="C10" s="6">
+        <v>15</v>
+      </c>
+      <c r="D10" s="12">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="E10" s="22">
+        <f t="shared" si="1"/>
+        <v>0.34242185699999994</v>
+      </c>
+      <c r="F10" s="26">
+        <f t="shared" si="2"/>
+        <v>22.942264418999997</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="B11" s="4">
+        <v>3</v>
+      </c>
+      <c r="C11" s="6">
+        <v>20</v>
+      </c>
+      <c r="D11" s="12">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
+      <c r="E11" s="22">
+        <f t="shared" si="1"/>
+        <v>0.25831824299999989</v>
+      </c>
+      <c r="F11" s="26">
+        <f t="shared" si="2"/>
+        <v>17.307322280999994</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="B12" s="4">
+        <v>4</v>
+      </c>
+      <c r="C12" s="6">
+        <v>8</v>
+      </c>
+      <c r="D12" s="12">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="E12" s="22">
+        <f t="shared" si="1"/>
+        <v>9.7435828500000002E-2</v>
+      </c>
+      <c r="F12" s="26">
+        <f t="shared" si="2"/>
+        <v>6.5282005095000004</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="5">
+        <v>5</v>
+      </c>
+      <c r="C13" s="7">
+        <v>2</v>
+      </c>
+      <c r="D13" s="12">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="E13" s="24">
+        <f t="shared" si="1"/>
+        <v>1.4700844299999998E-2</v>
+      </c>
+      <c r="F13" s="26">
+        <f t="shared" si="2"/>
+        <v>0.98495656809999987</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C14" s="17">
+        <f>SUM(C8:C13)</f>
+        <v>67</v>
+      </c>
+      <c r="D14" s="16">
+        <f>SUM(D8:D13)</f>
+        <v>144</v>
+      </c>
+      <c r="E14" s="18">
+        <f>SUM(E8:E13)</f>
+        <v>1</v>
+      </c>
+      <c r="F14" s="27">
+        <f>SUM(F8:F13)</f>
+        <v>67</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>29</v>
+      </c>
+      <c r="C17" s="19">
+        <f>D14/C14</f>
+        <v>2.1492537313432836</v>
+      </c>
+      <c r="D17" t="s">
+        <v>32</v>
+      </c>
+      <c r="E17">
+        <v>2.15</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>30</v>
+      </c>
+      <c r="C18" s="19">
+        <f>C17/5</f>
+        <v>0.42985074626865671</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>31</v>
+      </c>
+      <c r="C19" s="19">
+        <f>1-C18</f>
+        <v>0.57014925373134329</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B21" s="21"/>
+      <c r="C21" s="21"/>
+      <c r="D21" s="21"/>
+      <c r="E21" s="21"/>
+      <c r="F21" s="21"/>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B22" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C22" s="8"/>
+      <c r="F22" s="19"/>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>1</v>
+      </c>
+      <c r="C23" s="27">
+        <v>0</v>
+      </c>
+      <c r="D23" s="27">
+        <v>1</v>
+      </c>
+      <c r="E23" s="27">
+        <v>2</v>
+      </c>
+      <c r="F23" s="27">
+        <v>3</v>
+      </c>
+      <c r="G23" s="27">
+        <v>4</v>
+      </c>
+      <c r="H23" s="27">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>34</v>
+      </c>
+      <c r="C24" s="27">
+        <v>4.031336781900003</v>
+      </c>
+      <c r="D24" s="27">
+        <v>15.205919440500002</v>
+      </c>
+      <c r="E24" s="27">
+        <v>22.942264418999997</v>
+      </c>
+      <c r="F24" s="27">
+        <v>17.307322280999994</v>
+      </c>
+      <c r="G24" s="27">
+        <v>6.5282005095000004</v>
+      </c>
+      <c r="H24" s="27">
+        <v>0.98495656809999987</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C25" s="19"/>
+      <c r="F25" s="19"/>
+    </row>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C26" s="19"/>
+      <c r="F26" s="19"/>
+    </row>
+    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C27" s="19"/>
+      <c r="F27" s="19"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="B22:C22"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added more excel files
</commit_message>
<xml_diff>
--- a/business Stats/Book1.xlsx
+++ b/business Stats/Book1.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Ujwal\git\business Stats\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8D4F86E-6716-49DB-BBD6-5D8878E5184A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F9371AE-66EB-441E-A725-B70D6E7292B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{84D76DE3-8557-4722-B5C1-4893E077E0C2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{84D76DE3-8557-4722-B5C1-4893E077E0C2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="54">
   <si>
     <t>Calculate the correlation of the following data</t>
   </si>
@@ -255,13 +256,161 @@
   <si>
     <t>Fit the following data in Poisson Distribution.</t>
   </si>
+  <si>
+    <t>Let the mean &amp; SD of the normal distribution br 75 and 4 respectively.</t>
+  </si>
+  <si>
+    <t>Find out the following probabilities</t>
+  </si>
+  <si>
+    <r>
+      <t>i)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">                    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>P(x&lt;60)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>ii)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">                   </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>P(x&gt;65)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>iii)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>P(80&lt;=x&lt;=90)</t>
+    </r>
+  </si>
+  <si>
+    <t>SD</t>
+  </si>
+  <si>
+    <t>p(x&lt;60)</t>
+  </si>
+  <si>
+    <t>Working Expresson:</t>
+  </si>
+  <si>
+    <t>p(x&gt;65)</t>
+  </si>
+  <si>
+    <t>p(80&lt;=x&lt;=90)</t>
+  </si>
+  <si>
+    <t> P(60&lt;=x&lt;=84)</t>
+  </si>
+  <si>
+    <r>
+      <t>iv)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>P(60&lt;=x&lt;=84)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>i)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">                    </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">i)                                              </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">                    </t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.0000"/>
+    <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
   <fonts count="10" x14ac:knownFonts="1">
     <font>
@@ -586,7 +735,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -603,12 +752,6 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -617,26 +760,24 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -644,13 +785,10 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -682,10 +820,29 @@
       <alignment horizontal="left" vertical="center" indent="3"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2093,6 +2250,224 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>742950</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>446532</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ECAD33A6-0E52-40EA-8334-8C9478671BFC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:clrChange>
+            <a:clrFrom>
+              <a:srgbClr val="FFFFFF"/>
+            </a:clrFrom>
+            <a:clrTo>
+              <a:srgbClr val="FFFFFF">
+                <a:alpha val="0"/>
+              </a:srgbClr>
+            </a:clrTo>
+          </a:clrChange>
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1352550" y="1933575"/>
+          <a:ext cx="741807" cy="314325"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>276225</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0F373464-20ED-48CC-8BB3-7A5160ABBB06}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:clrChange>
+            <a:clrFrom>
+              <a:srgbClr val="FFFFFF"/>
+            </a:clrFrom>
+            <a:clrTo>
+              <a:srgbClr val="FFFFFF">
+                <a:alpha val="0"/>
+              </a:srgbClr>
+            </a:clrTo>
+          </a:clrChange>
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1924050" y="2305050"/>
+          <a:ext cx="1333500" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>333375</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>542925</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2C217B9A-B540-49BE-A339-B4016DEF69B3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+          <a:clrChange>
+            <a:clrFrom>
+              <a:srgbClr val="FFFFFF"/>
+            </a:clrFrom>
+            <a:clrTo>
+              <a:srgbClr val="FFFFFF">
+                <a:alpha val="0"/>
+              </a:srgbClr>
+            </a:clrTo>
+          </a:clrChange>
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1981200" y="2733675"/>
+          <a:ext cx="1009650" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -2406,26 +2781,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
+      <c r="F1" s="42"/>
+      <c r="G1" s="42"/>
+      <c r="H1" s="42"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="8"/>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
+      <c r="A2" s="42"/>
+      <c r="B2" s="42"/>
+      <c r="C2" s="42"/>
+      <c r="D2" s="42"/>
+      <c r="E2" s="42"/>
+      <c r="F2" s="42"/>
+      <c r="G2" s="42"/>
+      <c r="H2" s="42"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -2466,10 +2841,10 @@
       <c r="F4">
         <v>5</v>
       </c>
-      <c r="I4" s="9" t="s">
+      <c r="I4" s="43" t="s">
         <v>18</v>
       </c>
-      <c r="J4" s="8"/>
+      <c r="J4" s="42"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="J5" t="s">
@@ -2480,14 +2855,14 @@
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="8" t="s">
+      <c r="A6" s="42" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="8"/>
-      <c r="C6" s="8"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8"/>
+      <c r="B6" s="42"/>
+      <c r="C6" s="42"/>
+      <c r="D6" s="42"/>
+      <c r="E6" s="42"/>
+      <c r="F6" s="42"/>
       <c r="J6" t="s">
         <v>21</v>
       </c>
@@ -2496,22 +2871,22 @@
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="9" t="s">
+      <c r="A8" s="43" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="8"/>
-      <c r="F8" s="9" t="s">
+      <c r="B8" s="42"/>
+      <c r="F8" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="G8" s="8"/>
+      <c r="G8" s="42"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="8" t="s">
+      <c r="A9" s="42" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="8"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
+      <c r="B9" s="42"/>
+      <c r="C9" s="42"/>
+      <c r="D9" s="42"/>
       <c r="F9" t="s">
         <v>1</v>
       </c>
@@ -2520,10 +2895,10 @@
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="8"/>
-      <c r="B10" s="8"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
+      <c r="A10" s="42"/>
+      <c r="B10" s="42"/>
+      <c r="C10" s="42"/>
+      <c r="D10" s="42"/>
       <c r="F10">
         <v>2</v>
       </c>
@@ -2532,12 +2907,12 @@
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="8" t="s">
+      <c r="A11" s="42" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="8"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="8"/>
+      <c r="B11" s="42"/>
+      <c r="C11" s="42"/>
+      <c r="D11" s="42"/>
       <c r="F11">
         <v>7</v>
       </c>
@@ -2547,10 +2922,10 @@
       <c r="K11" s="2"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="8"/>
-      <c r="B12" s="8"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="8"/>
+      <c r="A12" s="42"/>
+      <c r="B12" s="42"/>
+      <c r="C12" s="42"/>
+      <c r="D12" s="42"/>
       <c r="F12">
         <v>6</v>
       </c>
@@ -2559,12 +2934,12 @@
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="8">
+      <c r="A13" s="42">
         <v>3</v>
       </c>
-      <c r="B13" s="8"/>
-      <c r="C13" s="8"/>
-      <c r="D13" s="8"/>
+      <c r="B13" s="42"/>
+      <c r="C13" s="42"/>
+      <c r="D13" s="42"/>
       <c r="F13">
         <v>3</v>
       </c>
@@ -2573,10 +2948,10 @@
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="8"/>
-      <c r="B14" s="8"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="8"/>
+      <c r="A14" s="42"/>
+      <c r="B14" s="42"/>
+      <c r="C14" s="42"/>
+      <c r="D14" s="42"/>
       <c r="F14">
         <v>4</v>
       </c>
@@ -2599,13 +2974,13 @@
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="8" t="s">
+      <c r="A19" s="42" t="s">
         <v>10</v>
       </c>
-      <c r="B19" s="8"/>
-      <c r="C19" s="8"/>
-      <c r="D19" s="8"/>
-      <c r="E19" s="8"/>
+      <c r="B19" s="42"/>
+      <c r="C19" s="42"/>
+      <c r="D19" s="42"/>
+      <c r="E19" s="42"/>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -2638,20 +3013,20 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="42" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
+      <c r="C2" s="42"/>
+      <c r="D2" s="42"/>
+      <c r="E2" s="42"/>
+      <c r="F2" s="42"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B3" s="8"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
+      <c r="B3" s="42"/>
+      <c r="C3" s="42"/>
+      <c r="D3" s="42"/>
+      <c r="E3" s="42"/>
+      <c r="F3" s="42"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
@@ -2694,32 +3069,32 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="42" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8"/>
+      <c r="C7" s="42"/>
+      <c r="D7" s="42"/>
+      <c r="E7" s="42"/>
+      <c r="F7" s="42"/>
+      <c r="G7" s="42"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="9" t="s">
+      <c r="A10" s="43" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="8"/>
-      <c r="E10" s="9" t="s">
+      <c r="B10" s="42"/>
+      <c r="E10" s="43" t="s">
         <v>17</v>
       </c>
-      <c r="F10" s="9"/>
+      <c r="F10" s="43"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="8" t="s">
+      <c r="A11" s="42" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="8"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="8"/>
+      <c r="B11" s="42"/>
+      <c r="C11" s="42"/>
+      <c r="D11" s="42"/>
       <c r="E11" t="s">
         <v>1</v>
       </c>
@@ -2728,12 +3103,12 @@
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="8" t="s">
+      <c r="A12" s="42" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="8"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="8"/>
+      <c r="B12" s="42"/>
+      <c r="C12" s="42"/>
+      <c r="D12" s="42"/>
       <c r="E12">
         <v>2</v>
       </c>
@@ -2742,12 +3117,12 @@
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="8" t="s">
+      <c r="A13" s="42" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="8"/>
-      <c r="C13" s="8"/>
-      <c r="D13" s="8"/>
+      <c r="B13" s="42"/>
+      <c r="C13" s="42"/>
+      <c r="D13" s="42"/>
       <c r="E13">
         <v>7</v>
       </c>
@@ -2780,14 +3155,14 @@
       </c>
     </row>
     <row r="18" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E18" s="8" t="s">
+      <c r="E18" s="42" t="s">
         <v>23</v>
       </c>
-      <c r="F18" s="8"/>
+      <c r="F18" s="42"/>
     </row>
     <row r="19" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E19" s="8"/>
-      <c r="F19" s="8"/>
+      <c r="E19" s="42"/>
+      <c r="F19" s="42"/>
     </row>
     <row r="20" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E20" t="s">
@@ -2799,32 +3174,32 @@
       </c>
     </row>
     <row r="36" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B36" s="9" t="s">
+      <c r="B36" s="43" t="s">
         <v>9</v>
       </c>
-      <c r="C36" s="8"/>
+      <c r="C36" s="42"/>
     </row>
     <row r="37" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B37" s="8" t="s">
+      <c r="B37" s="42" t="s">
         <v>25</v>
       </c>
-      <c r="C37" s="8"/>
+      <c r="C37" s="42"/>
       <c r="D37" t="s">
         <v>26</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="B2:F3"/>
+    <mergeCell ref="B7:G7"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A11:D11"/>
+    <mergeCell ref="A12:D12"/>
     <mergeCell ref="A13:D13"/>
     <mergeCell ref="E10:F10"/>
     <mergeCell ref="E18:F19"/>
     <mergeCell ref="B36:C36"/>
     <mergeCell ref="B37:C37"/>
-    <mergeCell ref="B2:F3"/>
-    <mergeCell ref="B7:G7"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A11:D11"/>
-    <mergeCell ref="A12:D12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2836,7 +3211,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68AC71F3-EDAC-4C28-A1D6-182EE705764F}">
   <dimension ref="A1:H77"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
+    <sheetView view="pageLayout" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
       <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
@@ -2847,108 +3222,107 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="31" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="37" t="s">
+      <c r="A2" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="38">
+      <c r="B2" s="33">
         <v>0</v>
       </c>
-      <c r="C2" s="38">
+      <c r="C2" s="33">
         <v>1</v>
       </c>
-      <c r="D2" s="38">
+      <c r="D2" s="33">
         <v>2</v>
       </c>
-      <c r="E2" s="38">
+      <c r="E2" s="33">
         <v>3</v>
       </c>
-      <c r="F2" s="38">
+      <c r="F2" s="33">
         <v>4</v>
       </c>
-      <c r="G2" s="38">
+      <c r="G2" s="33">
         <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="39" t="s">
+      <c r="A3" s="34" t="s">
         <v>27</v>
       </c>
-      <c r="B3" s="40">
+      <c r="B3" s="35">
         <v>3</v>
       </c>
-      <c r="C3" s="40">
+      <c r="C3" s="35">
         <v>7</v>
       </c>
-      <c r="D3" s="40">
+      <c r="D3" s="35">
         <v>10</v>
       </c>
-      <c r="E3" s="40">
+      <c r="E3" s="35">
         <v>15</v>
       </c>
-      <c r="F3" s="40">
+      <c r="F3" s="35">
         <v>8</v>
       </c>
-      <c r="G3" s="40">
+      <c r="G3" s="35">
         <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="36"/>
+      <c r="A4" s="31"/>
       <c r="H4" s="5"/>
     </row>
     <row r="5" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="36"/>
+      <c r="A5" s="31"/>
     </row>
     <row r="6" spans="1:8" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="A6" s="36" t="s">
+      <c r="A6" s="31" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="47">
+      <c r="A7" s="41">
         <v>1</v>
       </c>
-      <c r="B7" s="46"/>
-      <c r="C7" s="46"/>
+      <c r="B7" s="45"/>
+      <c r="C7" s="45"/>
     </row>
     <row r="8" spans="1:8" ht="21" x14ac:dyDescent="0.25">
-      <c r="A8" s="41"/>
+      <c r="A8" s="36"/>
     </row>
     <row r="9" spans="1:8" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="41" t="s">
+      <c r="A9" s="36" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="42"/>
+      <c r="A10" s="37"/>
     </row>
     <row r="11" spans="1:8" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="43" t="s">
+      <c r="A11" s="38" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A12" s="44" t="s">
+      <c r="A12" s="39" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="21.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="45"/>
+      <c r="A13" s="40"/>
     </row>
     <row r="14" spans="1:8" ht="21.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="45"/>
+      <c r="A14" s="40"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B15" s="15"/>
-      <c r="C15" s="16"/>
-      <c r="D15" s="16"/>
-      <c r="E15" s="16"/>
-      <c r="F15" s="16"/>
+      <c r="C15" s="12"/>
+      <c r="D15" s="12"/>
+      <c r="E15" s="12"/>
+      <c r="F15" s="12"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B16" s="3"/>
@@ -2971,39 +3345,39 @@
       <c r="B18" s="1"/>
     </row>
     <row r="19" spans="1:8" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="11" t="s">
+      <c r="B19" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C19" s="25" t="s">
+      <c r="C19" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="D19" s="26" t="s">
+      <c r="D19" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="E19" s="26" t="s">
+      <c r="E19" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="F19" s="27" t="s">
+      <c r="F19" s="23" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="B20" s="10">
+      <c r="B20" s="8">
         <v>0</v>
       </c>
-      <c r="C20" s="21">
+      <c r="C20" s="17">
         <v>10</v>
       </c>
-      <c r="D20" s="22">
-        <f>B20*C20</f>
+      <c r="D20" s="18">
+        <f t="shared" ref="D20:D25" si="0">B20*C20</f>
         <v>0</v>
       </c>
-      <c r="E20" s="23">
-        <f>_xlfn.BINOM.DIST(B20,5,0.43,0)</f>
+      <c r="E20" s="19">
+        <f t="shared" ref="E20:E25" si="1">_xlfn.BINOM.DIST(B20,5,0.43,0)</f>
         <v>6.016920570000004E-2</v>
       </c>
-      <c r="F20" s="24">
-        <f>67*E20</f>
+      <c r="F20" s="20">
+        <f t="shared" ref="F20:F25" si="2">67*E20</f>
         <v>4.031336781900003</v>
       </c>
     </row>
@@ -3011,19 +3385,19 @@
       <c r="B21" s="6">
         <v>1</v>
       </c>
-      <c r="C21" s="17">
+      <c r="C21" s="13">
         <v>12</v>
       </c>
       <c r="D21" s="7">
-        <f>B21*C21</f>
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="E21" s="18">
-        <f>_xlfn.BINOM.DIST(B21,5,0.43,0)</f>
+      <c r="E21" s="14">
+        <f t="shared" si="1"/>
         <v>0.22695402150000005</v>
       </c>
-      <c r="F21" s="20">
-        <f>67*E21</f>
+      <c r="F21" s="16">
+        <f t="shared" si="2"/>
         <v>15.205919440500002</v>
       </c>
     </row>
@@ -3031,106 +3405,106 @@
       <c r="B22" s="6">
         <v>2</v>
       </c>
-      <c r="C22" s="17">
+      <c r="C22" s="13">
         <v>15</v>
       </c>
       <c r="D22" s="7">
-        <f>B22*C22</f>
+        <f t="shared" si="0"/>
         <v>30</v>
       </c>
-      <c r="E22" s="18">
-        <f>_xlfn.BINOM.DIST(B22,5,0.43,0)</f>
+      <c r="E22" s="14">
+        <f t="shared" si="1"/>
         <v>0.34242185699999994</v>
       </c>
-      <c r="F22" s="20">
-        <f>67*E22</f>
+      <c r="F22" s="16">
+        <f t="shared" si="2"/>
         <v>22.942264418999997</v>
       </c>
-      <c r="G22" s="16"/>
-      <c r="H22" s="16"/>
+      <c r="G22" s="12"/>
+      <c r="H22" s="12"/>
     </row>
     <row r="23" spans="1:8" ht="19.5" x14ac:dyDescent="0.25">
       <c r="B23" s="6">
         <v>3</v>
       </c>
-      <c r="C23" s="17">
+      <c r="C23" s="13">
         <v>20</v>
       </c>
       <c r="D23" s="7">
-        <f>B23*C23</f>
+        <f t="shared" si="0"/>
         <v>60</v>
       </c>
-      <c r="E23" s="18">
-        <f>_xlfn.BINOM.DIST(B23,5,0.43,0)</f>
+      <c r="E23" s="14">
+        <f t="shared" si="1"/>
         <v>0.25831824299999989</v>
       </c>
-      <c r="F23" s="20">
-        <f>67*E23</f>
+      <c r="F23" s="16">
+        <f t="shared" si="2"/>
         <v>17.307322280999994</v>
       </c>
-      <c r="G23" s="16"/>
-      <c r="H23" s="16"/>
+      <c r="G23" s="12"/>
+      <c r="H23" s="12"/>
     </row>
     <row r="24" spans="1:8" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A24" s="3"/>
       <c r="B24" s="6">
         <v>4</v>
       </c>
-      <c r="C24" s="17">
+      <c r="C24" s="13">
         <v>8</v>
       </c>
       <c r="D24" s="7">
-        <f>B24*C24</f>
+        <f t="shared" si="0"/>
         <v>32</v>
       </c>
-      <c r="E24" s="18">
-        <f>_xlfn.BINOM.DIST(B24,5,0.43,0)</f>
+      <c r="E24" s="14">
+        <f t="shared" si="1"/>
         <v>9.7435828500000002E-2</v>
       </c>
-      <c r="F24" s="20">
-        <f>67*E24</f>
+      <c r="F24" s="16">
+        <f t="shared" si="2"/>
         <v>6.5282005095000004</v>
       </c>
       <c r="G24" s="3"/>
       <c r="H24" s="3"/>
     </row>
     <row r="25" spans="1:8" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="28">
+      <c r="B25" s="24">
         <v>5</v>
       </c>
-      <c r="C25" s="29">
+      <c r="C25" s="25">
         <v>2</v>
       </c>
-      <c r="D25" s="30">
-        <f>B25*C25</f>
+      <c r="D25" s="26">
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="E25" s="31">
-        <f>_xlfn.BINOM.DIST(B25,5,0.43,0)</f>
+      <c r="E25" s="27">
+        <f t="shared" si="1"/>
         <v>1.4700844299999998E-2</v>
       </c>
-      <c r="F25" s="32">
-        <f>67*E25</f>
+      <c r="F25" s="28">
+        <f t="shared" si="2"/>
         <v>0.98495656809999987</v>
       </c>
       <c r="G25" s="5"/>
       <c r="H25" s="5"/>
     </row>
     <row r="26" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="12"/>
-      <c r="C26" s="26">
+      <c r="B26" s="10"/>
+      <c r="C26" s="22">
         <f>SUM(C20:C25)</f>
         <v>67</v>
       </c>
-      <c r="D26" s="26">
+      <c r="D26" s="22">
         <f>SUM(D20:D25)</f>
         <v>144</v>
       </c>
-      <c r="E26" s="33">
+      <c r="E26" s="29">
         <f>SUM(E20:E25)</f>
         <v>1</v>
       </c>
-      <c r="F26" s="34">
+      <c r="F26" s="30">
         <f>SUM(F20:F25)</f>
         <v>67</v>
       </c>
@@ -3139,7 +3513,7 @@
       <c r="B29" t="s">
         <v>29</v>
       </c>
-      <c r="C29" s="13">
+      <c r="C29" s="11">
         <f>D26/C26</f>
         <v>2.1492537313432836</v>
       </c>
@@ -3154,7 +3528,7 @@
       <c r="B30" t="s">
         <v>30</v>
       </c>
-      <c r="C30" s="13">
+      <c r="C30" s="11">
         <f>C29/5</f>
         <v>0.42985074626865671</v>
       </c>
@@ -3163,45 +3537,38 @@
       <c r="B31" t="s">
         <v>31</v>
       </c>
-      <c r="C31" s="13">
+      <c r="C31" s="11">
         <f>1-C30</f>
         <v>0.57014925373134329</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B33" s="14"/>
-      <c r="C33" s="14"/>
-      <c r="D33" s="14"/>
-      <c r="E33" s="14"/>
-      <c r="F33" s="14"/>
-    </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B34" s="35" t="s">
+      <c r="B34" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="C34" s="35"/>
-      <c r="F34" s="13"/>
+      <c r="C34" s="44"/>
+      <c r="F34" s="11"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B35" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C35" s="19">
+      <c r="C35" s="15">
         <v>0</v>
       </c>
-      <c r="D35" s="19">
+      <c r="D35" s="15">
         <v>1</v>
       </c>
-      <c r="E35" s="19">
+      <c r="E35" s="15">
         <v>2</v>
       </c>
-      <c r="F35" s="19">
+      <c r="F35" s="15">
         <v>3</v>
       </c>
-      <c r="G35" s="19">
+      <c r="G35" s="15">
         <v>4</v>
       </c>
-      <c r="H35" s="19">
+      <c r="H35" s="15">
         <v>5</v>
       </c>
     </row>
@@ -3209,128 +3576,127 @@
       <c r="B36" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="C36" s="19">
+      <c r="C36" s="15">
         <v>4.031336781900003</v>
       </c>
-      <c r="D36" s="19">
+      <c r="D36" s="15">
         <v>15.205919440500002</v>
       </c>
-      <c r="E36" s="19">
+      <c r="E36" s="15">
         <v>22.942264418999997</v>
       </c>
-      <c r="F36" s="19">
+      <c r="F36" s="15">
         <v>17.307322280999994</v>
       </c>
-      <c r="G36" s="19">
+      <c r="G36" s="15">
         <v>6.5282005095000004</v>
       </c>
-      <c r="H36" s="19">
+      <c r="H36" s="15">
         <v>0.98495656809999987</v>
       </c>
     </row>
     <row r="42" spans="1:8" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="36" t="s">
+      <c r="A42" s="31" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="43" spans="1:8" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="37" t="s">
+      <c r="A43" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="B43" s="38">
+      <c r="B43" s="33">
         <v>0</v>
       </c>
-      <c r="C43" s="38">
+      <c r="C43" s="33">
         <v>1</v>
       </c>
-      <c r="D43" s="38">
+      <c r="D43" s="33">
         <v>2</v>
       </c>
-      <c r="E43" s="38">
+      <c r="E43" s="33">
         <v>3</v>
       </c>
-      <c r="F43" s="38">
+      <c r="F43" s="33">
         <v>4</v>
       </c>
-      <c r="G43" s="38">
+      <c r="G43" s="33">
         <v>5</v>
       </c>
     </row>
     <row r="44" spans="1:8" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="39" t="s">
+      <c r="A44" s="34" t="s">
         <v>27</v>
       </c>
-      <c r="B44" s="40">
+      <c r="B44" s="35">
         <v>3</v>
       </c>
-      <c r="C44" s="40">
+      <c r="C44" s="35">
         <v>7</v>
       </c>
-      <c r="D44" s="40">
+      <c r="D44" s="35">
         <v>10</v>
       </c>
-      <c r="E44" s="40">
+      <c r="E44" s="35">
         <v>15</v>
       </c>
-      <c r="F44" s="40">
+      <c r="F44" s="35">
         <v>8</v>
       </c>
-      <c r="G44" s="40">
+      <c r="G44" s="35">
         <v>2</v>
       </c>
     </row>
     <row r="45" spans="1:8" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="A45" s="36"/>
+      <c r="A45" s="31"/>
       <c r="H45" s="5"/>
     </row>
     <row r="46" spans="1:8" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="A46" s="36"/>
+      <c r="A46" s="31"/>
     </row>
     <row r="47" spans="1:8" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="A47" s="36" t="s">
+      <c r="A47" s="31" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="48" spans="1:8" ht="21" x14ac:dyDescent="0.25">
-      <c r="A48" s="47">
+      <c r="A48" s="41">
         <v>1</v>
       </c>
-      <c r="B48" s="46"/>
-      <c r="C48" s="46"/>
+      <c r="B48" s="45"/>
+      <c r="C48" s="45"/>
     </row>
     <row r="49" spans="1:8" ht="21" x14ac:dyDescent="0.25">
-      <c r="A49" s="41"/>
+      <c r="A49" s="36"/>
     </row>
     <row r="50" spans="1:8" ht="21" x14ac:dyDescent="0.25">
-      <c r="A50" s="41" t="s">
+      <c r="A50" s="36" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A51" s="42"/>
+      <c r="A51" s="37"/>
     </row>
     <row r="52" spans="1:8" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="A52" s="43" t="s">
+      <c r="A52" s="38" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="53" spans="1:8" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A53" s="44" t="s">
+      <c r="A53" s="39" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="54" spans="1:8" ht="21.75" x14ac:dyDescent="0.25">
-      <c r="A54" s="45"/>
+      <c r="A54" s="40"/>
     </row>
     <row r="55" spans="1:8" ht="21.75" x14ac:dyDescent="0.25">
-      <c r="A55" s="45"/>
+      <c r="A55" s="40"/>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B56" s="15"/>
-      <c r="C56" s="16"/>
-      <c r="D56" s="16"/>
-      <c r="E56" s="16"/>
-      <c r="F56" s="16"/>
+      <c r="C56" s="12"/>
+      <c r="D56" s="12"/>
+      <c r="E56" s="12"/>
+      <c r="F56" s="12"/>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B57" s="3"/>
@@ -3353,38 +3719,38 @@
       <c r="B59" s="1"/>
     </row>
     <row r="60" spans="1:8" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B60" s="11" t="s">
+      <c r="B60" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C60" s="25" t="s">
+      <c r="C60" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="D60" s="26" t="s">
+      <c r="D60" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="E60" s="26" t="s">
+      <c r="E60" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="F60" s="27" t="s">
+      <c r="F60" s="23" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="61" spans="1:8" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="B61" s="10">
+      <c r="B61" s="8">
         <v>0</v>
       </c>
-      <c r="C61" s="21">
+      <c r="C61" s="17">
         <v>10</v>
       </c>
-      <c r="D61" s="22">
-        <f>B61*C61</f>
+      <c r="D61" s="18">
+        <f t="shared" ref="D61:D66" si="3">B61*C61</f>
         <v>0</v>
       </c>
-      <c r="E61" s="23">
+      <c r="E61" s="19">
         <f>_xlfn.POISSON.DIST(B61,2.15,0)</f>
         <v>0.11648415777349697</v>
       </c>
-      <c r="F61" s="24">
+      <c r="F61" s="20">
         <f>67*E61</f>
         <v>7.8044385708242965</v>
       </c>
@@ -3393,19 +3759,19 @@
       <c r="B62" s="6">
         <v>1</v>
       </c>
-      <c r="C62" s="17">
+      <c r="C62" s="13">
         <v>12</v>
       </c>
       <c r="D62" s="7">
-        <f>B62*C62</f>
+        <f t="shared" si="3"/>
         <v>12</v>
       </c>
-      <c r="E62" s="23">
-        <f t="shared" ref="E62:E66" si="0">_xlfn.POISSON.DIST(B62,2.15,0)</f>
+      <c r="E62" s="19">
+        <f t="shared" ref="E62:E66" si="4">_xlfn.POISSON.DIST(B62,2.15,0)</f>
         <v>0.25044093921301847</v>
       </c>
-      <c r="F62" s="20">
-        <f t="shared" ref="F62:F66" si="1">67*E62</f>
+      <c r="F62" s="16">
+        <f t="shared" ref="F62:F66" si="5">67*E62</f>
         <v>16.779542927272239</v>
       </c>
     </row>
@@ -3413,106 +3779,106 @@
       <c r="B63" s="6">
         <v>2</v>
       </c>
-      <c r="C63" s="17">
+      <c r="C63" s="13">
         <v>15</v>
       </c>
       <c r="D63" s="7">
-        <f>B63*C63</f>
+        <f t="shared" si="3"/>
         <v>30</v>
       </c>
-      <c r="E63" s="23">
-        <f t="shared" si="0"/>
+      <c r="E63" s="19">
+        <f t="shared" si="4"/>
         <v>0.2692240096539949</v>
       </c>
-      <c r="F63" s="20">
-        <f t="shared" si="1"/>
+      <c r="F63" s="16">
+        <f t="shared" si="5"/>
         <v>18.038008646817659</v>
       </c>
-      <c r="G63" s="16"/>
-      <c r="H63" s="16"/>
+      <c r="G63" s="12"/>
+      <c r="H63" s="12"/>
     </row>
     <row r="64" spans="1:8" ht="19.5" x14ac:dyDescent="0.25">
       <c r="B64" s="6">
         <v>3</v>
       </c>
-      <c r="C64" s="17">
+      <c r="C64" s="13">
         <v>20</v>
       </c>
       <c r="D64" s="7">
-        <f>B64*C64</f>
+        <f t="shared" si="3"/>
         <v>60</v>
       </c>
-      <c r="E64" s="23">
-        <f t="shared" si="0"/>
+      <c r="E64" s="19">
+        <f t="shared" si="4"/>
         <v>0.19294387358536297</v>
       </c>
-      <c r="F64" s="20">
-        <f t="shared" si="1"/>
+      <c r="F64" s="16">
+        <f t="shared" si="5"/>
         <v>12.927239530219319</v>
       </c>
-      <c r="G64" s="16"/>
-      <c r="H64" s="16"/>
+      <c r="G64" s="12"/>
+      <c r="H64" s="12"/>
     </row>
     <row r="65" spans="1:8" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A65" s="3"/>
       <c r="B65" s="6">
         <v>4</v>
       </c>
-      <c r="C65" s="17">
+      <c r="C65" s="13">
         <v>8</v>
       </c>
       <c r="D65" s="7">
-        <f>B65*C65</f>
+        <f t="shared" si="3"/>
         <v>32</v>
       </c>
-      <c r="E65" s="23">
-        <f t="shared" si="0"/>
+      <c r="E65" s="19">
+        <f t="shared" si="4"/>
         <v>0.10370733205213264</v>
       </c>
-      <c r="F65" s="20">
-        <f t="shared" si="1"/>
+      <c r="F65" s="16">
+        <f t="shared" si="5"/>
         <v>6.9483912474928875</v>
       </c>
       <c r="G65" s="3"/>
       <c r="H65" s="3"/>
     </row>
     <row r="66" spans="1:8" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B66" s="28">
+      <c r="B66" s="24">
         <v>5</v>
       </c>
-      <c r="C66" s="29">
+      <c r="C66" s="25">
         <v>2</v>
       </c>
-      <c r="D66" s="30">
-        <f>B66*C66</f>
+      <c r="D66" s="26">
+        <f t="shared" si="3"/>
         <v>10</v>
       </c>
-      <c r="E66" s="23">
-        <f t="shared" si="0"/>
+      <c r="E66" s="19">
+        <f t="shared" si="4"/>
         <v>4.4594152782417018E-2</v>
       </c>
-      <c r="F66" s="32">
-        <f t="shared" si="1"/>
+      <c r="F66" s="28">
+        <f t="shared" si="5"/>
         <v>2.98780823642194</v>
       </c>
       <c r="G66" s="5"/>
       <c r="H66" s="5"/>
     </row>
     <row r="67" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B67" s="12"/>
-      <c r="C67" s="26">
+      <c r="B67" s="10"/>
+      <c r="C67" s="22">
         <f>SUM(C61:C66)</f>
         <v>67</v>
       </c>
-      <c r="D67" s="26">
+      <c r="D67" s="22">
         <f>SUM(D61:D66)</f>
         <v>144</v>
       </c>
-      <c r="E67" s="33">
+      <c r="E67" s="29">
         <f>SUM(E61:E66)</f>
         <v>0.97739446506042293</v>
       </c>
-      <c r="F67" s="34">
+      <c r="F67" s="30">
         <f>SUM(F61:F66)</f>
         <v>65.485429159048337</v>
       </c>
@@ -3521,7 +3887,7 @@
       <c r="B70" t="s">
         <v>29</v>
       </c>
-      <c r="C70" s="13">
+      <c r="C70" s="11">
         <f>D67/C67</f>
         <v>2.1492537313432836</v>
       </c>
@@ -3533,45 +3899,38 @@
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C71" s="13"/>
+      <c r="C71" s="11"/>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C72" s="13"/>
-    </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B74" s="14"/>
-      <c r="C74" s="14"/>
-      <c r="D74" s="14"/>
-      <c r="E74" s="14"/>
-      <c r="F74" s="14"/>
+      <c r="C72" s="11"/>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B75" s="35" t="s">
+      <c r="B75" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="C75" s="35"/>
-      <c r="F75" s="13"/>
+      <c r="C75" s="44"/>
+      <c r="F75" s="11"/>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B76" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C76" s="19">
+      <c r="C76" s="15">
         <v>0</v>
       </c>
-      <c r="D76" s="19">
+      <c r="D76" s="15">
         <v>1</v>
       </c>
-      <c r="E76" s="19">
+      <c r="E76" s="15">
         <v>2</v>
       </c>
-      <c r="F76" s="19">
+      <c r="F76" s="15">
         <v>3</v>
       </c>
-      <c r="G76" s="19">
+      <c r="G76" s="15">
         <v>4</v>
       </c>
-      <c r="H76" s="19">
+      <c r="H76" s="15">
         <v>5</v>
       </c>
     </row>
@@ -3579,22 +3938,22 @@
       <c r="B77" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="C77" s="19" t="s">
+      <c r="C77" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="D77" s="19">
+      <c r="D77" s="15">
         <v>7.8044385708242965</v>
       </c>
-      <c r="E77" s="19">
+      <c r="E77" s="15">
         <v>16.779542927272239</v>
       </c>
-      <c r="F77" s="19">
+      <c r="F77" s="15">
         <v>18.038008646817659</v>
       </c>
-      <c r="G77" s="19">
+      <c r="G77" s="15">
         <v>12.927239530219319</v>
       </c>
-      <c r="H77" s="19">
+      <c r="H77" s="15">
         <v>6.9483912474928875</v>
       </c>
     </row>
@@ -3613,4 +3972,204 @@
   </headerFooter>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D7078FA-1A72-4D50-BCE6-1E804DF4C344}">
+  <dimension ref="B3:J23"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="15.5703125" customWidth="1"/>
+    <col min="3" max="4" width="12" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B3" s="47" t="s">
+        <v>40</v>
+      </c>
+      <c r="C3" s="46"/>
+      <c r="D3" s="46"/>
+      <c r="E3" s="46"/>
+      <c r="F3" s="46"/>
+      <c r="G3" s="46"/>
+      <c r="H3" s="46"/>
+      <c r="I3" s="46"/>
+      <c r="J3" s="46"/>
+    </row>
+    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B4" s="47" t="s">
+        <v>41</v>
+      </c>
+      <c r="C4" s="46"/>
+      <c r="D4" s="46"/>
+      <c r="E4" s="46"/>
+      <c r="F4" s="46"/>
+      <c r="G4" s="46"/>
+      <c r="H4" s="46"/>
+      <c r="I4" s="46"/>
+      <c r="J4" s="46"/>
+    </row>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B5" s="48" t="s">
+        <v>42</v>
+      </c>
+      <c r="C5" s="48"/>
+      <c r="D5" s="48"/>
+      <c r="E5" s="48"/>
+      <c r="F5" s="46"/>
+      <c r="G5" s="46"/>
+      <c r="H5" s="46"/>
+      <c r="I5" s="46"/>
+      <c r="J5" s="46"/>
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B6" s="48" t="s">
+        <v>43</v>
+      </c>
+      <c r="C6" s="48"/>
+      <c r="D6" s="48"/>
+      <c r="E6" s="48"/>
+      <c r="F6" s="46"/>
+      <c r="G6" s="46"/>
+      <c r="H6" s="46"/>
+      <c r="I6" s="46"/>
+      <c r="J6" s="46"/>
+    </row>
+    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B7" s="48" t="s">
+        <v>44</v>
+      </c>
+      <c r="C7" s="48"/>
+      <c r="D7" s="48"/>
+      <c r="E7" s="48"/>
+    </row>
+    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B8" s="48" t="s">
+        <v>51</v>
+      </c>
+      <c r="C8" s="48"/>
+      <c r="D8" s="48"/>
+      <c r="E8" s="48"/>
+    </row>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B10" s="43" t="s">
+        <v>47</v>
+      </c>
+      <c r="C10" s="42"/>
+      <c r="D10" s="42"/>
+    </row>
+    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B11" s="48" t="s">
+        <v>53</v>
+      </c>
+      <c r="C11" s="48"/>
+      <c r="D11" s="48"/>
+      <c r="E11" s="48"/>
+    </row>
+    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B12" s="48"/>
+      <c r="C12" s="48"/>
+      <c r="D12" s="48"/>
+      <c r="E12" s="48"/>
+    </row>
+    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B13" s="48" t="s">
+        <v>52</v>
+      </c>
+      <c r="C13" s="49"/>
+      <c r="D13" s="49"/>
+      <c r="E13" s="49"/>
+    </row>
+    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B14" s="48"/>
+      <c r="C14" s="49"/>
+      <c r="D14" s="49"/>
+      <c r="E14" s="49"/>
+    </row>
+    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B15" s="42"/>
+      <c r="C15" s="48"/>
+      <c r="D15" s="48"/>
+      <c r="E15" s="48"/>
+    </row>
+    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B16" s="42"/>
+      <c r="C16" s="48"/>
+      <c r="D16" s="48"/>
+      <c r="E16" s="48"/>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>29</v>
+      </c>
+      <c r="C18">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>45</v>
+      </c>
+      <c r="C19">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>46</v>
+      </c>
+      <c r="C20">
+        <f>NORMDIST(60,75,4,1)</f>
+        <v>8.841728520080376E-5</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>48</v>
+      </c>
+      <c r="C21">
+        <f>1-NORMDIST(65,75,4,1)</f>
+        <v>0.99379033467422384</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>49</v>
+      </c>
+      <c r="C22">
+        <f>NORMDIST(90,75,4,1)-NORMDIST(80,75,4,1)</f>
+        <v>0.10556135638165443</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>50</v>
+      </c>
+      <c r="C23">
+        <f>NORMDIST(84,75,4,1)-NORMDIST(60,75,4,1)</f>
+        <v>0.98768711005975451</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="10">
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="C15:E16"/>
+    <mergeCell ref="B11:E12"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="C13:E14"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="B10:D10"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>